<commit_message>
added statusbericht1, new view in mockup, completed entries of Workjournal
</commit_message>
<xml_diff>
--- a/Dokumentation/IPT71_Journal&Planung.xlsx
+++ b/Dokumentation/IPT71_Journal&Planung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sluz-my.sharepoint.com/personal/benjamin_maier_sluz_ch/Documents/BBZW_2/Sem_2/IPT71/chipslyfans/Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{E8630097-044A-4CD1-9566-22D5144B9F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{080A8E38-1156-497F-BC1F-4B0B377A186F}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{E8630097-044A-4CD1-9566-22D5144B9F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D09BE44-6017-4743-BBC2-BF1CD0BA2970}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <r>
       <rPr>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>API-Struktur, Dokumentation, UI-Komponenten, Dokumentation</t>
+  </si>
+  <si>
+    <t>Fertigstellung in %</t>
+  </si>
+  <si>
+    <t>Zeitplan: 100%, Anforderungen: 100%, Grundgerüst Frontend: 20% (Register&amp;LoginView fertig), Mockup zu 70 % fertig, User-System: 20%(Backend für User&amp;Post fertig)</t>
+  </si>
+  <si>
+    <t>Grundgerüst Frontend: 30%(NotificationsView fertig), User-System: 35%(Einloggen und register über Backend möglich ,JSON-WebToken wird generiert), Mockup: 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grundgerüst Frontend: 40%, User-System: 40%(HomeView kann Post laden), Mockup: 80%, Dokumentation: 100% </t>
   </si>
 </sst>
 </file>
@@ -257,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -328,13 +340,7 @@
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
@@ -347,6 +353,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="9" x14ac:dyDescent="0.2"/>
@@ -665,38 +674,38 @@
     <col min="4" max="4" width="5.83203125" style="16" customWidth="1"/>
     <col min="5" max="6" width="33.83203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="28" style="16" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="16" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.33203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="96.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-    </row>
-    <row r="2" spans="1:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+    </row>
+    <row r="2" spans="1:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -718,57 +727,59 @@
       <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="24"/>
-      <c r="AQ2" s="24"/>
-      <c r="AR2" s="24"/>
-      <c r="AS2" s="24"/>
-      <c r="AT2" s="24"/>
-      <c r="AU2" s="24"/>
-      <c r="AV2" s="24"/>
-      <c r="AW2" s="24"/>
-      <c r="AX2" s="24"/>
-      <c r="AY2" s="24"/>
-      <c r="AZ2" s="24"/>
-      <c r="BA2" s="24"/>
-      <c r="BB2" s="24"/>
-      <c r="BC2" s="24"/>
-      <c r="BD2" s="24"/>
-      <c r="BE2" s="24"/>
-      <c r="BF2" s="24"/>
+      <c r="H2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="23"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="23"/>
+      <c r="AW2" s="23"/>
+      <c r="AX2" s="23"/>
+      <c r="AY2" s="23"/>
+      <c r="AZ2" s="23"/>
+      <c r="BA2" s="23"/>
+      <c r="BB2" s="23"/>
+      <c r="BC2" s="23"/>
+      <c r="BD2" s="23"/>
+      <c r="BE2" s="23"/>
+      <c r="BF2" s="23"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
@@ -786,57 +797,57 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="24"/>
-      <c r="AO3" s="24"/>
-      <c r="AP3" s="24"/>
-      <c r="AQ3" s="24"/>
-      <c r="AR3" s="24"/>
-      <c r="AS3" s="24"/>
-      <c r="AT3" s="24"/>
-      <c r="AU3" s="24"/>
-      <c r="AV3" s="24"/>
-      <c r="AW3" s="24"/>
-      <c r="AX3" s="24"/>
-      <c r="AY3" s="24"/>
-      <c r="AZ3" s="24"/>
-      <c r="BA3" s="24"/>
-      <c r="BB3" s="24"/>
-      <c r="BC3" s="24"/>
-      <c r="BD3" s="24"/>
-      <c r="BE3" s="24"/>
-      <c r="BF3" s="24"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23"/>
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
@@ -854,57 +865,57 @@
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="24"/>
-      <c r="AO4" s="24"/>
-      <c r="AP4" s="24"/>
-      <c r="AQ4" s="24"/>
-      <c r="AR4" s="24"/>
-      <c r="AS4" s="24"/>
-      <c r="AT4" s="24"/>
-      <c r="AU4" s="24"/>
-      <c r="AV4" s="24"/>
-      <c r="AW4" s="24"/>
-      <c r="AX4" s="24"/>
-      <c r="AY4" s="24"/>
-      <c r="AZ4" s="24"/>
-      <c r="BA4" s="24"/>
-      <c r="BB4" s="24"/>
-      <c r="BC4" s="24"/>
-      <c r="BD4" s="24"/>
-      <c r="BE4" s="24"/>
-      <c r="BF4" s="24"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AT4" s="23"/>
+      <c r="AU4" s="23"/>
+      <c r="AV4" s="23"/>
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23"/>
+      <c r="BA4" s="23"/>
+      <c r="BB4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="23"/>
+      <c r="BF4" s="23"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
@@ -922,57 +933,57 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="24"/>
-      <c r="AO5" s="24"/>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24"/>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="24"/>
-      <c r="AT5" s="24"/>
-      <c r="AU5" s="24"/>
-      <c r="AV5" s="24"/>
-      <c r="AW5" s="24"/>
-      <c r="AX5" s="24"/>
-      <c r="AY5" s="24"/>
-      <c r="AZ5" s="24"/>
-      <c r="BA5" s="24"/>
-      <c r="BB5" s="24"/>
-      <c r="BC5" s="24"/>
-      <c r="BD5" s="24"/>
-      <c r="BE5" s="24"/>
-      <c r="BF5" s="24"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="23"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="23"/>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="23"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="23"/>
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="23"/>
+      <c r="AV5" s="23"/>
+      <c r="AW5" s="23"/>
+      <c r="AX5" s="23"/>
+      <c r="AY5" s="23"/>
+      <c r="AZ5" s="23"/>
+      <c r="BA5" s="23"/>
+      <c r="BB5" s="23"/>
+      <c r="BC5" s="23"/>
+      <c r="BD5" s="23"/>
+      <c r="BE5" s="23"/>
+      <c r="BF5" s="23"/>
     </row>
     <row r="6" spans="1:58" ht="11.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22">
@@ -990,57 +1001,57 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="24"/>
-      <c r="AM6" s="24"/>
-      <c r="AN6" s="24"/>
-      <c r="AO6" s="24"/>
-      <c r="AP6" s="24"/>
-      <c r="AQ6" s="24"/>
-      <c r="AR6" s="24"/>
-      <c r="AS6" s="24"/>
-      <c r="AT6" s="24"/>
-      <c r="AU6" s="24"/>
-      <c r="AV6" s="24"/>
-      <c r="AW6" s="24"/>
-      <c r="AX6" s="24"/>
-      <c r="AY6" s="24"/>
-      <c r="AZ6" s="24"/>
-      <c r="BA6" s="24"/>
-      <c r="BB6" s="24"/>
-      <c r="BC6" s="24"/>
-      <c r="BD6" s="24"/>
-      <c r="BE6" s="24"/>
-      <c r="BF6" s="24"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="23"/>
+      <c r="AR6" s="23"/>
+      <c r="AS6" s="23"/>
+      <c r="AT6" s="23"/>
+      <c r="AU6" s="23"/>
+      <c r="AV6" s="23"/>
+      <c r="AW6" s="23"/>
+      <c r="AX6" s="23"/>
+      <c r="AY6" s="23"/>
+      <c r="AZ6" s="23"/>
+      <c r="BA6" s="23"/>
+      <c r="BB6" s="23"/>
+      <c r="BC6" s="23"/>
+      <c r="BD6" s="23"/>
+      <c r="BE6" s="23"/>
+      <c r="BF6" s="23"/>
     </row>
     <row r="7" spans="1:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1056,57 +1067,57 @@
         <v>9</v>
       </c>
       <c r="G7" s="19"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="24"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="24"/>
-      <c r="AG7" s="24"/>
-      <c r="AH7" s="24"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="24"/>
-      <c r="AK7" s="24"/>
-      <c r="AL7" s="24"/>
-      <c r="AM7" s="24"/>
-      <c r="AN7" s="24"/>
-      <c r="AO7" s="24"/>
-      <c r="AP7" s="24"/>
-      <c r="AQ7" s="24"/>
-      <c r="AR7" s="24"/>
-      <c r="AS7" s="24"/>
-      <c r="AT7" s="24"/>
-      <c r="AU7" s="24"/>
-      <c r="AV7" s="24"/>
-      <c r="AW7" s="24"/>
-      <c r="AX7" s="24"/>
-      <c r="AY7" s="24"/>
-      <c r="AZ7" s="24"/>
-      <c r="BA7" s="24"/>
-      <c r="BB7" s="24"/>
-      <c r="BC7" s="24"/>
-      <c r="BD7" s="24"/>
-      <c r="BE7" s="24"/>
-      <c r="BF7" s="24"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+      <c r="AG7" s="23"/>
+      <c r="AH7" s="23"/>
+      <c r="AI7" s="23"/>
+      <c r="AJ7" s="23"/>
+      <c r="AK7" s="23"/>
+      <c r="AL7" s="23"/>
+      <c r="AM7" s="23"/>
+      <c r="AN7" s="23"/>
+      <c r="AO7" s="23"/>
+      <c r="AP7" s="23"/>
+      <c r="AQ7" s="23"/>
+      <c r="AR7" s="23"/>
+      <c r="AS7" s="23"/>
+      <c r="AT7" s="23"/>
+      <c r="AU7" s="23"/>
+      <c r="AV7" s="23"/>
+      <c r="AW7" s="23"/>
+      <c r="AX7" s="23"/>
+      <c r="AY7" s="23"/>
+      <c r="AZ7" s="23"/>
+      <c r="BA7" s="23"/>
+      <c r="BB7" s="23"/>
+      <c r="BC7" s="23"/>
+      <c r="BD7" s="23"/>
+      <c r="BE7" s="23"/>
+      <c r="BF7" s="23"/>
     </row>
     <row r="8" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
@@ -1122,57 +1133,57 @@
         <v>9</v>
       </c>
       <c r="G8" s="19"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="24"/>
-      <c r="AI8" s="24"/>
-      <c r="AJ8" s="24"/>
-      <c r="AK8" s="24"/>
-      <c r="AL8" s="24"/>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="24"/>
-      <c r="AO8" s="24"/>
-      <c r="AP8" s="24"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="24"/>
-      <c r="AS8" s="24"/>
-      <c r="AT8" s="24"/>
-      <c r="AU8" s="24"/>
-      <c r="AV8" s="24"/>
-      <c r="AW8" s="24"/>
-      <c r="AX8" s="24"/>
-      <c r="AY8" s="24"/>
-      <c r="AZ8" s="24"/>
-      <c r="BA8" s="24"/>
-      <c r="BB8" s="24"/>
-      <c r="BC8" s="24"/>
-      <c r="BD8" s="24"/>
-      <c r="BE8" s="24"/>
-      <c r="BF8" s="24"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="23"/>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="23"/>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="23"/>
+      <c r="AO8" s="23"/>
+      <c r="AP8" s="23"/>
+      <c r="AQ8" s="23"/>
+      <c r="AR8" s="23"/>
+      <c r="AS8" s="23"/>
+      <c r="AT8" s="23"/>
+      <c r="AU8" s="23"/>
+      <c r="AV8" s="23"/>
+      <c r="AW8" s="23"/>
+      <c r="AX8" s="23"/>
+      <c r="AY8" s="23"/>
+      <c r="AZ8" s="23"/>
+      <c r="BA8" s="23"/>
+      <c r="BB8" s="23"/>
+      <c r="BC8" s="23"/>
+      <c r="BD8" s="23"/>
+      <c r="BE8" s="23"/>
+      <c r="BF8" s="23"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
@@ -1190,40 +1201,40 @@
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-    </row>
-    <row r="10" spans="1:58" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="18"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+    </row>
+    <row r="10" spans="1:58" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22">
         <v>12</v>
       </c>
       <c r="B10" s="22">
         <v>25</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>45733</v>
       </c>
       <c r="D10" s="22">
         <v>3</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="23"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:58" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
@@ -1241,30 +1252,32 @@
       <c r="E11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-    </row>
-    <row r="12" spans="1:58" ht="27" x14ac:dyDescent="0.15">
+      <c r="H11" s="28">
+        <v>1</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+    </row>
+    <row r="12" spans="1:58" ht="45" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>14</v>
       </c>
@@ -1281,25 +1294,29 @@
         <v>15</v>
       </c>
       <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-    </row>
-    <row r="13" spans="1:58" ht="18" x14ac:dyDescent="0.15">
+      <c r="G12" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+    </row>
+    <row r="13" spans="1:58" ht="54" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>15</v>
       </c>
@@ -1316,25 +1333,29 @@
         <v>16</v>
       </c>
       <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-    </row>
-    <row r="14" spans="1:58" ht="18" x14ac:dyDescent="0.15">
+      <c r="G13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+    </row>
+    <row r="14" spans="1:58" ht="36" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>16</v>
       </c>
@@ -1351,23 +1372,27 @@
         <v>17</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
+      <c r="G14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
     </row>
     <row r="15" spans="1:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
@@ -1383,22 +1408,22 @@
         <v>8</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
     </row>
     <row r="16" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
@@ -1414,22 +1439,22 @@
         <v>8</v>
       </c>
       <c r="G16" s="19"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
     </row>
     <row r="17" spans="1:23" ht="18" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
@@ -1449,22 +1474,22 @@
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
     </row>
     <row r="18" spans="1:23" ht="18" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
@@ -1484,22 +1509,22 @@
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
     </row>
     <row r="19" spans="1:23" ht="18" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
@@ -1519,22 +1544,22 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
     </row>
     <row r="20" spans="1:23" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
@@ -1554,22 +1579,22 @@
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
     </row>
     <row r="21" spans="1:23" ht="12.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
@@ -1589,22 +1614,22 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
     </row>
     <row r="22" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
@@ -1622,22 +1647,22 @@
         <v>10</v>
       </c>
       <c r="G22" s="20"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
     </row>
     <row r="23" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
@@ -1655,22 +1680,22 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="18"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
     </row>
     <row r="24" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
@@ -1688,24 +1713,24 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-    </row>
-    <row r="25" spans="1:23" ht="11.1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H24" s="21"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+    </row>
+    <row r="25" spans="1:23" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>27</v>
       </c>
@@ -1721,22 +1746,22 @@
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
     </row>
     <row r="26" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
@@ -1752,22 +1777,22 @@
         <v>7</v>
       </c>
       <c r="G26" s="19"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
     </row>
     <row r="28" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F28" s="16" t="s">

</xml_diff>